<commit_message>
small % calculation mistake fixed
</commit_message>
<xml_diff>
--- a/NSAS/stf/stfTableStochastic_Deterministic.xlsx
+++ b/NSAS/stf/stfTableStochastic_Deterministic.xlsx
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,11 +1137,11 @@
         <v>1965073.91330642</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" ref="N4:N8" si="0">(L4-L$2)/L$2</f>
+        <f>(L4-L$2)/L$2</f>
         <v>-6.2739639097881453E-2</v>
       </c>
       <c r="O4" s="4">
-        <f t="shared" ref="O4:O8" si="1">(H4-405000)/405000</f>
+        <f t="shared" ref="O4:O8" si="0">(H4-405000)/405000</f>
         <v>-0.15000000000000244</v>
       </c>
     </row>
@@ -1186,11 +1186,11 @@
         <v>1804761.6988706</v>
       </c>
       <c r="N5" s="4">
+        <f t="shared" ref="N4:N8" si="1">(L5-L$2)/L$2</f>
+        <v>-9.8936283779356649E-2</v>
+      </c>
+      <c r="O5" s="4">
         <f t="shared" si="0"/>
-        <v>-9.8936283779356649E-2</v>
-      </c>
-      <c r="O5" s="4">
-        <f t="shared" si="1"/>
         <v>0.14999999999991606</v>
       </c>
     </row>
@@ -1235,11 +1235,11 @@
         <v>2483573.9497907101</v>
       </c>
       <c r="N6" s="4">
+        <f t="shared" si="1"/>
+        <v>4.0002376680273989E-2</v>
+      </c>
+      <c r="O6" s="4">
         <f t="shared" si="0"/>
-        <v>4.0002376680273989E-2</v>
-      </c>
-      <c r="O6" s="4">
-        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
@@ -1284,11 +1284,11 @@
         <v>1884082.1502082399</v>
       </c>
       <c r="N7" s="4">
+        <f t="shared" si="1"/>
+        <v>-8.0771527492037046E-2</v>
+      </c>
+      <c r="O7" s="4">
         <f t="shared" si="0"/>
-        <v>-8.0771527492037046E-2</v>
-      </c>
-      <c r="O7" s="4">
-        <f t="shared" si="1"/>
         <v>-2.2820099314421782E-9</v>
       </c>
     </row>
@@ -1333,11 +1333,11 @@
         <v>1627864.0529229599</v>
       </c>
       <c r="N8" s="4">
+        <f>(L8-L$2)/L$2</f>
+        <v>-0.14144873308257119</v>
+      </c>
+      <c r="O8" s="4">
         <f t="shared" si="0"/>
-        <v>-0.14144873308257119</v>
-      </c>
-      <c r="O8" s="4">
-        <f t="shared" si="1"/>
         <v>0.49667829693760002</v>
       </c>
     </row>
@@ -1566,7 +1566,7 @@
         <v>-0.12871235862371369</v>
       </c>
       <c r="O14" s="4">
-        <f t="shared" ref="O13:O17" si="3">(H14-H$25)/H$25</f>
+        <f t="shared" ref="O14:O17" si="3">(H14-H$25)/H$25</f>
         <v>0.14999999997098024</v>
       </c>
     </row>

</xml_diff>